<commit_message>
feat: checkpoint spt pph
</commit_message>
<xml_diff>
--- a/database/data/kapKjs.xlsx
+++ b/database/data/kapKjs.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDREK\PT SAMUDRA EDUKASI TEKNOLOGI\Backend_Coretaxify\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05F36B8-AE3C-4E78-9041-15D649620FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46C2882-E9B5-4005-A947-F72504F1E0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KAP - KJS - Pembayaran" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="y94bue0susICWanviBsQ7WD/h6M64eMpwcVbPLQ2RGo="/>
     </ext>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
   <si>
     <t>-</t>
   </si>
@@ -358,6 +367,12 @@
   </si>
   <si>
     <t>PPN</t>
+  </si>
+  <si>
+    <t>411121-100</t>
+  </si>
+  <si>
+    <t>PPH21</t>
   </si>
 </sst>
 </file>
@@ -404,12 +419,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +644,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1213,6 +1229,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>